<commit_message>
Enhance scheme details display by adding more location and scheme information.
Replit-Commit-Author: Agent
Replit-Commit-Session-Id: b8968fc8-6d12-48e8-bcf8-35f0a41cd3f4
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/3dbb296a-ff24-4257-a265-ba725ae84225/db996cca-040c-4e24-b299-bbff01db0aa9.jpg
</commit_message>
<xml_diff>
--- a/attached_assets/scheme_level_datalink_report.xlsx
+++ b/attached_assets/scheme_level_datalink_report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\OneDrive\Pictures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1000001_{8A4E4714-4EC6-E245-9B88-DA20E1D464FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1000001_{748B5575-51BF-0440-931D-12CC96771076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="2" xr2:uid="{0BA389E0-F6F9-4736-8426-92409BD6B05C}"/>
   </bookViews>
@@ -9401,8 +9401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C264139-9F10-460E-997C-1DDE2CC71A99}">
   <dimension ref="A1:X63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T32" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:W63"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H57" sqref="H57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>